<commit_message>
Update Jinja2 custom env with block trimming and newline configurations
</commit_message>
<xml_diff>
--- a/examples/example3/catalog_template.xlsx
+++ b/examples/example3/catalog_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\apps\jinjaxcat\examples\example3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9262D027-98C5-4CCB-AEBC-931EE9D30F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B4304E-37DC-4F6F-ACFD-50142F30CAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8805" yWindow="4575" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="3525" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Material</t>
   </si>
@@ -41,19 +41,39 @@
     <t>EAN</t>
   </si>
   <si>
-    <t>{% for article in articles_json %}{{article['SUPPLIER_AID']}}{{split}}{% endfor %}</t>
-  </si>
-  <si>
-    <t>{% for article in articles_json %}{{article['DESCRIPTION_LONG']}}{{split}}{% endfor %}</t>
-  </si>
-  <si>
-    <t>{% for article in articles_json %}{{article['PRICE_AMOUNT']}}{{split}}{% endfor %}</t>
-  </si>
-  <si>
-    <t>{% for article in articles_json %}EUR{{split}}{% endfor %}</t>
-  </si>
-  <si>
-    <t>{% for article in articles_json %}{{article['EAN']}}{{split}}{% endfor %}</t>
+    <t>{% for article in articles_json %}
+{{article['SUPPLIER_AID']}}
+{{split}}
+{% endfor %}</t>
+  </si>
+  <si>
+    <t>{% for article in articles_json %}
+{{article['DESCRIPTION_LONG']}}
+{{split}}
+{% endfor %}</t>
+  </si>
+  <si>
+    <t>{% for article in articles_json %}
+{{article['EAN']}}
+{{split}}
+{% endfor %}</t>
+  </si>
+  <si>
+    <t>{% for article in articles_json %}
+{{article['PRICE_AMOUNT']|int}}
+{{split}}
+{% endfor %}</t>
+  </si>
+  <si>
+    <t>{% for article in articles_json %}
+EUR{{split}}
+{% endfor %}</t>
+  </si>
+  <si>
+    <t>{% for article in articles_json %}
+{{ article['DESCRIPTION_SHORT']|upper }} is priced at {{ article['PRICE_AMOUNT'] }} with VAT.
+{{split}}
+{% endfor %}</t>
   </si>
 </sst>
 </file>
@@ -113,10 +133,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,50 +425,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356EB7F7-D963-4DDC-BBE0-EE7D9720E832}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="29.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -451,25 +479,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF06C2EF-F354-4478-AFF3-9846179843D2}">
-  <dimension ref="B2:B3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="90.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>6</v>
+    <row r="2" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>